<commit_message>
Prettified diagram, added requirements
</commit_message>
<xml_diff>
--- a/app4mc.waters.fmtv.challenge.requirements/Waters2019Reqs.xlsx
+++ b/app4mc.waters.fmtv.challenge.requirements/Waters2019Reqs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salomem/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janste/git/waters-challenge-2019/app4mc.waters.fmtv.challenge.requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A26603A-A9D8-8740-833F-062B9CD75617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F3788B-4BD0-674B-A343-B980DBD35F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="1320" windowWidth="33520" windowHeight="22680" xr2:uid="{7B98FAFD-CFA2-0D46-A189-A24C3A6EEAE5}"/>
+    <workbookView xWindow="1560" yWindow="5760" windowWidth="33520" windowHeight="22680" xr2:uid="{7B98FAFD-CFA2-0D46-A189-A24C3A6EEAE5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -44,27 +44,12 @@
     <t>The system shall avoid vulnerable road users</t>
   </si>
   <si>
-    <t xml:space="preserve"> The system shall detect all vulnerable road users</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The system shall be able to combine different sensors to identify vulnerable road users</t>
-  </si>
-  <si>
     <t>1.1.1</t>
   </si>
   <si>
     <t>1.1</t>
   </si>
   <si>
-    <t>1.3.2.1 The system shall detect road boundaries and shape of each lane</t>
-  </si>
-  <si>
-    <t>1.3.2.2 The system shall detect other vehicles or obstacles in the next lane</t>
-  </si>
-  <si>
-    <t>1.3.2.3 The system shall switch road lanes within 2s if the vulnerable user is detected within a dangerous zone</t>
-  </si>
-  <si>
     <t>The system shall perform an emergency manoeuvre to avoid vulnerable road users</t>
   </si>
   <si>
@@ -77,9 +62,6 @@
     <t>1.2.1.1</t>
   </si>
   <si>
-    <t>The system shall break within 2s if the vulnerable user is detected within a dangerous zone</t>
-  </si>
-  <si>
     <t>The system shall break to avoid a vulnerable road user</t>
   </si>
   <si>
@@ -128,29 +110,45 @@
     <t>The system shall translate the trajectory into vehicle commands</t>
   </si>
   <si>
-    <t xml:space="preserve"> The system shall follow the defined trajectory</t>
-  </si>
-  <si>
     <t>The system shall define a trajectory through a set of way points</t>
   </si>
   <si>
     <t>The system shall drive through a pre-determined set of way points</t>
+  </si>
+  <si>
+    <t>The system shall detect road boundaries and shape of each lane</t>
+  </si>
+  <si>
+    <t>The system shall detect other vehicles or obstacles in the next lane</t>
+  </si>
+  <si>
+    <t>The system shall follow the defined trajectory</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>The system shall be able to differentiate between a vulnerable road user and different items in the environment</t>
+  </si>
+  <si>
+    <t>The system shall be able to combine different sensors to identify vulnerable road users</t>
+  </si>
+  <si>
+    <t>The system shall detect all vulnerable road users</t>
+  </si>
+  <si>
+    <t>The system shall switch road lanes within 800ms after a vulnerable road user is detected within a dangerous zone</t>
+  </si>
+  <si>
+    <t>The system shall break within 500ms after the vulnerable user is detected within a dangerous zone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -163,13 +161,46 @@
       <name val="Helvetica"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -184,13 +215,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,163 +541,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EB6FC7-7B12-6A40-928E-4D999F2A9B43}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="74.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2">
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="B15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="2">
-        <v>2</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="C20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>